<commit_message>
update: change menu regarding to the AccountType of the login user
</commit_message>
<xml_diff>
--- a/Templates/er01ir.xlsx
+++ b/Templates/er01ir.xlsx
@@ -1,27 +1,112 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\Evaluation\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38370" windowHeight="13080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Worksheet!$A$1:$M$84</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+  <si>
+    <t>Boss</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Collaborator</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Name:</t>
+  </si>
+  <si>
+    <t>CHAN TAI MAN, PETER</t>
+  </si>
+  <si>
+    <t>Department:</t>
+  </si>
+  <si>
+    <t>Position:</t>
+  </si>
+  <si>
+    <t>As you review this report, remember the following two items:</t>
+  </si>
+  <si>
+    <t>1. Take a balance view</t>
+  </si>
+  <si>
+    <t>Straight feedback is a priceless gift. Don't spend time guessing who gave you low scores or hostility toward people who responded.
+Thank them for taking the time to give you feedback, then use the data in a balanced effective way to improve your competency.</t>
+  </si>
+  <si>
+    <t>2. Make an action plan</t>
+  </si>
+  <si>
+    <t>Use the data a part of your continued effort to become a better performer</t>
+  </si>
+  <si>
+    <t>Subordinate</t>
+  </si>
+  <si>
+    <t>Staff ID:</t>
+  </si>
+  <si>
+    <t>Evaluation Code:</t>
+  </si>
+  <si>
+    <t>RAD</t>
+  </si>
+  <si>
+    <t>SENIOR PROGRAMMER</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -32,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -40,18 +125,203 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +368,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +403,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +611,827 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="23"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="C3" s="23"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="M13" s="7"/>
+    </row>
+    <row r="14" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:13" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="19"/>
+    </row>
+    <row r="16" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="8"/>
+      <c r="M16" s="7"/>
+    </row>
+    <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17" s="7"/>
+    </row>
+    <row r="18" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="10"/>
+    </row>
+    <row r="19" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="14"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="14"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="14"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="14"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="14"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="14"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="14"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="14"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="14"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="14"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="14"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="14"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="14"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K58" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L58" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M58" s="12"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="22"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="12"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="14"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="14"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="14"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="14"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+      <c r="K64" s="14"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="14"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="14"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="14"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+      <c r="K66" s="14"/>
+      <c r="L66" s="14"/>
+      <c r="M66" s="14"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="14"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="14"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="14"/>
+      <c r="L68" s="14"/>
+      <c r="M68" s="14"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="14"/>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="14"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="14"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="14"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="14"/>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="14"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="14"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="14"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
+      <c r="H72" s="14"/>
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="14"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="14"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="14"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
+      <c r="H74" s="14"/>
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14"/>
+      <c r="L74" s="14"/>
+      <c r="M74" s="14"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="14"/>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
+      <c r="H75" s="14"/>
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="14"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="14"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
+      <c r="H76" s="14"/>
+      <c r="I76" s="14"/>
+      <c r="J76" s="14"/>
+      <c r="K76" s="14"/>
+      <c r="L76" s="14"/>
+      <c r="M76" s="14"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="14"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
+      <c r="H77" s="14"/>
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="14"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="14"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="14"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+      <c r="K78" s="14"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="14"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="14"/>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="14"/>
+      <c r="H79" s="14"/>
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
+      <c r="M79" s="14"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14"/>
+      <c r="G80" s="14"/>
+      <c r="H80" s="14"/>
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+      <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="14"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="14"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="14"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="14"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="14"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="14"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <mergeCells count="4">
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="B58:I58"/>
+    <mergeCell ref="B59:I59"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="1.1653125" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="76" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Calibri,Bold"&amp;18QODIVA 360 Degree Feedback
+Individual Report</oddHeader>
+    <oddFooter>&amp;RPrivate and confidential</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bug Fixed and Update
pageview
fixed: go to the last page button
fixed: the refresh button

All pages
update: menu item

update: require evaluation code on submit
-individual report page
-process-gen-eva-proposal page

update: Status column change to EvaProQtnStatusCode
-process-gen-eva-proposal page

Individual Report
add: total and average value
add: pdf report properties
</commit_message>
<xml_diff>
--- a/Templates/er01ir.xlsx
+++ b/Templates/er01ir.xlsx
@@ -16,14 +16,14 @@
     <sheet name="Chart" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Worksheet!$A$1:$M$84</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Worksheet!$A$1:$M$85</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Boss</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Use the data a part of your continued effort to become a better performer</t>
   </si>
   <si>
-    <t>Subordinate</t>
-  </si>
-  <si>
     <t>Staff ID:</t>
   </si>
   <si>
@@ -90,6 +87,15 @@
   </si>
   <si>
     <t>SENIOR PROGRAMMER</t>
+  </si>
+  <si>
+    <t>Subordinate      Avg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Marks </t>
+  </si>
+  <si>
+    <t>Average Marks</t>
   </si>
 </sst>
 </file>
@@ -261,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -280,6 +286,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -305,8 +314,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,30 +627,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M84"/>
+  <dimension ref="A2:M85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="23"/>
+        <v>18</v>
+      </c>
+      <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="C3" s="23"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -652,7 +667,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -660,7 +675,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -700,21 +715,21 @@
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="20"/>
     </row>
     <row r="16" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
@@ -728,18 +743,18 @@
       <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="10"/>
@@ -928,69 +943,73 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
-      <c r="I58" s="22"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="22"/>
+      <c r="I58" s="23"/>
       <c r="J58" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K58" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K58" s="11" t="s">
-        <v>0</v>
-      </c>
       <c r="L58" s="11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="M58" s="12"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="22"/>
+      <c r="B59" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="25"/>
+      <c r="D59" s="25"/>
+      <c r="E59" s="25"/>
+      <c r="F59" s="25"/>
+      <c r="G59" s="25"/>
+      <c r="H59" s="25"/>
+      <c r="I59" s="26"/>
       <c r="J59" s="11"/>
       <c r="K59" s="11"/>
       <c r="L59" s="11"/>
-      <c r="M59" s="12"/>
+      <c r="M59" s="11"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
-      <c r="L60" s="14"/>
-      <c r="M60" s="14"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
-      <c r="L62" s="14"/>
-      <c r="M62" s="14"/>
+      <c r="A60" s="13"/>
+      <c r="B60" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="25"/>
+      <c r="D60" s="25"/>
+      <c r="E60" s="25"/>
+      <c r="F60" s="25"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="25"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="12"/>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="14"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="14"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="14"/>
@@ -1322,12 +1341,28 @@
       <c r="L84" s="14"/>
       <c r="M84" s="14"/>
     </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85" s="14"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="14"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A18:J18"/>
     <mergeCell ref="A15:M15"/>
     <mergeCell ref="B58:I58"/>
+    <mergeCell ref="B60:I60"/>
     <mergeCell ref="B59:I59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.1653125" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>